<commit_message>
anh tuan nb + kim long
</commit_message>
<xml_diff>
--- a/5. WS/1. Bộ phận bảo hành/1. Thực hiện sửa chữa bảo hành/nam2022/Thang11/2.XulyBH/XLBH2211_AnhTuanNB.xlsx
+++ b/5. WS/1. Bộ phận bảo hành/1. Thực hiện sửa chữa bảo hành/nam2022/Thang11/2.XulyBH/XLBH2211_AnhTuanNB.xlsx
@@ -814,6 +814,30 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -831,30 +855,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1165,8 +1165,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X115"/>
   <sheetViews>
-    <sheetView showZeros="0" tabSelected="1" topLeftCell="M1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="S11" sqref="S11"/>
+    <sheetView showZeros="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1198,41 +1198,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="74"/>
-      <c r="B1" s="74"/>
-      <c r="C1" s="74"/>
-      <c r="D1" s="74"/>
-      <c r="E1" s="74"/>
-      <c r="F1" s="74"/>
-      <c r="G1" s="74"/>
-      <c r="H1" s="74"/>
-      <c r="I1" s="74"/>
-      <c r="J1" s="74"/>
-      <c r="K1" s="74"/>
-      <c r="L1" s="74"/>
-      <c r="M1" s="74"/>
-      <c r="N1" s="74"/>
-      <c r="O1" s="74"/>
-      <c r="P1" s="74"/>
-      <c r="Q1" s="74"/>
-      <c r="R1" s="74"/>
-      <c r="S1" s="74"/>
-      <c r="T1" s="74"/>
-      <c r="U1" s="74"/>
-      <c r="V1" s="74"/>
+      <c r="A1" s="82"/>
+      <c r="B1" s="82"/>
+      <c r="C1" s="82"/>
+      <c r="D1" s="82"/>
+      <c r="E1" s="82"/>
+      <c r="F1" s="82"/>
+      <c r="G1" s="82"/>
+      <c r="H1" s="82"/>
+      <c r="I1" s="82"/>
+      <c r="J1" s="82"/>
+      <c r="K1" s="82"/>
+      <c r="L1" s="82"/>
+      <c r="M1" s="82"/>
+      <c r="N1" s="82"/>
+      <c r="O1" s="82"/>
+      <c r="P1" s="82"/>
+      <c r="Q1" s="82"/>
+      <c r="R1" s="82"/>
+      <c r="S1" s="82"/>
+      <c r="T1" s="82"/>
+      <c r="U1" s="82"/>
+      <c r="V1" s="82"/>
       <c r="W1" s="44"/>
     </row>
     <row r="2" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="75" t="s">
+      <c r="A2" s="83" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="76"/>
-      <c r="C2" s="76"/>
-      <c r="D2" s="76"/>
-      <c r="E2" s="77" t="s">
+      <c r="B2" s="84"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="85" t="s">
         <v>63</v>
       </c>
-      <c r="F2" s="77"/>
+      <c r="F2" s="85"/>
       <c r="G2" s="4"/>
       <c r="H2" s="20"/>
       <c r="I2" s="48"/>
@@ -1277,58 +1277,58 @@
       <c r="W3" s="26"/>
     </row>
     <row r="4" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="78" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="73" t="s">
+      <c r="A4" s="86" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="81" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="73"/>
-      <c r="D4" s="73"/>
-      <c r="E4" s="73"/>
-      <c r="F4" s="73"/>
-      <c r="G4" s="73"/>
-      <c r="H4" s="73"/>
-      <c r="I4" s="73"/>
-      <c r="J4" s="73" t="s">
+      <c r="C4" s="81"/>
+      <c r="D4" s="81"/>
+      <c r="E4" s="81"/>
+      <c r="F4" s="81"/>
+      <c r="G4" s="81"/>
+      <c r="H4" s="81"/>
+      <c r="I4" s="81"/>
+      <c r="J4" s="81" t="s">
         <v>6</v>
       </c>
-      <c r="K4" s="73" t="s">
+      <c r="K4" s="81" t="s">
         <v>11</v>
       </c>
-      <c r="L4" s="73"/>
-      <c r="M4" s="79" t="s">
+      <c r="L4" s="81"/>
+      <c r="M4" s="78" t="s">
         <v>42</v>
       </c>
-      <c r="N4" s="79" t="s">
+      <c r="N4" s="78" t="s">
         <v>10</v>
       </c>
-      <c r="O4" s="79" t="s">
+      <c r="O4" s="78" t="s">
         <v>7</v>
       </c>
-      <c r="P4" s="84" t="s">
+      <c r="P4" s="76" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="79" t="s">
+      <c r="Q4" s="78" t="s">
         <v>39</v>
       </c>
-      <c r="R4" s="79" t="s">
+      <c r="R4" s="78" t="s">
         <v>53</v>
       </c>
-      <c r="S4" s="86" t="s">
+      <c r="S4" s="80" t="s">
         <v>54</v>
       </c>
       <c r="T4" s="26"/>
-      <c r="U4" s="73" t="s">
+      <c r="U4" s="81" t="s">
         <v>39</v>
       </c>
-      <c r="V4" s="73" t="s">
+      <c r="V4" s="81" t="s">
         <v>53</v>
       </c>
       <c r="W4" s="45"/>
     </row>
     <row r="5" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="78"/>
+      <c r="A5" s="86"/>
       <c r="B5" s="71" t="s">
         <v>1</v>
       </c>
@@ -1353,23 +1353,23 @@
       <c r="I5" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="73"/>
+      <c r="J5" s="81"/>
       <c r="K5" s="71" t="s">
         <v>12</v>
       </c>
       <c r="L5" s="71" t="s">
         <v>13</v>
       </c>
-      <c r="M5" s="80"/>
-      <c r="N5" s="80"/>
-      <c r="O5" s="80"/>
-      <c r="P5" s="85"/>
-      <c r="Q5" s="80"/>
-      <c r="R5" s="80"/>
-      <c r="S5" s="86"/>
+      <c r="M5" s="79"/>
+      <c r="N5" s="79"/>
+      <c r="O5" s="79"/>
+      <c r="P5" s="77"/>
+      <c r="Q5" s="79"/>
+      <c r="R5" s="79"/>
+      <c r="S5" s="80"/>
       <c r="T5" s="26"/>
-      <c r="U5" s="73"/>
-      <c r="V5" s="73"/>
+      <c r="U5" s="81"/>
+      <c r="V5" s="81"/>
       <c r="W5" s="45"/>
     </row>
     <row r="6" spans="1:23" s="11" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -1425,7 +1425,7 @@
       </c>
       <c r="S6" s="67"/>
       <c r="T6" s="72"/>
-      <c r="U6" s="81" t="s">
+      <c r="U6" s="73" t="s">
         <v>18</v>
       </c>
       <c r="V6" s="3" t="s">
@@ -1456,7 +1456,7 @@
       <c r="R7" s="62"/>
       <c r="S7" s="67"/>
       <c r="T7" s="72"/>
-      <c r="U7" s="82"/>
+      <c r="U7" s="74"/>
       <c r="V7" s="3" t="s">
         <v>35</v>
       </c>
@@ -1485,7 +1485,7 @@
       <c r="R8" s="62"/>
       <c r="S8" s="67"/>
       <c r="T8" s="72"/>
-      <c r="U8" s="82"/>
+      <c r="U8" s="74"/>
       <c r="V8" s="3" t="s">
         <v>21</v>
       </c>
@@ -1514,7 +1514,7 @@
       <c r="R9" s="62"/>
       <c r="S9" s="67"/>
       <c r="T9" s="72"/>
-      <c r="U9" s="82"/>
+      <c r="U9" s="74"/>
       <c r="V9" s="3" t="s">
         <v>51</v>
       </c>
@@ -1543,7 +1543,7 @@
       <c r="R10" s="62"/>
       <c r="S10" s="67"/>
       <c r="T10" s="72"/>
-      <c r="U10" s="82"/>
+      <c r="U10" s="74"/>
       <c r="V10" s="3" t="s">
         <v>31</v>
       </c>
@@ -1572,7 +1572,7 @@
       <c r="R11" s="62"/>
       <c r="S11" s="67"/>
       <c r="T11" s="72"/>
-      <c r="U11" s="82"/>
+      <c r="U11" s="74"/>
       <c r="V11" s="3" t="s">
         <v>30</v>
       </c>
@@ -1601,7 +1601,7 @@
       <c r="R12" s="62"/>
       <c r="S12" s="67"/>
       <c r="T12" s="72"/>
-      <c r="U12" s="81" t="s">
+      <c r="U12" s="73" t="s">
         <v>19</v>
       </c>
       <c r="V12" s="3" t="s">
@@ -1632,7 +1632,7 @@
       <c r="R13" s="62"/>
       <c r="S13" s="67"/>
       <c r="T13" s="72"/>
-      <c r="U13" s="82"/>
+      <c r="U13" s="74"/>
       <c r="V13" s="3" t="s">
         <v>37</v>
       </c>
@@ -1661,7 +1661,7 @@
       <c r="R14" s="62"/>
       <c r="S14" s="67"/>
       <c r="T14" s="72"/>
-      <c r="U14" s="82"/>
+      <c r="U14" s="74"/>
       <c r="V14" s="3" t="s">
         <v>36</v>
       </c>
@@ -1690,7 +1690,7 @@
       <c r="R15" s="62"/>
       <c r="S15" s="67"/>
       <c r="T15" s="13"/>
-      <c r="U15" s="82"/>
+      <c r="U15" s="74"/>
       <c r="V15" s="3" t="s">
         <v>24</v>
       </c>
@@ -1719,7 +1719,7 @@
       <c r="R16" s="62"/>
       <c r="S16" s="67"/>
       <c r="T16" s="13"/>
-      <c r="U16" s="83"/>
+      <c r="U16" s="75"/>
       <c r="V16" s="3" t="s">
         <v>25</v>
       </c>
@@ -3436,13 +3436,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="U6:U11"/>
-    <mergeCell ref="U12:U16"/>
-    <mergeCell ref="P4:P5"/>
-    <mergeCell ref="Q4:Q5"/>
-    <mergeCell ref="R4:R5"/>
-    <mergeCell ref="S4:S5"/>
-    <mergeCell ref="U4:U5"/>
     <mergeCell ref="V4:V5"/>
     <mergeCell ref="A1:V1"/>
     <mergeCell ref="A2:D2"/>
@@ -3454,6 +3447,13 @@
     <mergeCell ref="M4:M5"/>
     <mergeCell ref="N4:N5"/>
     <mergeCell ref="O4:O5"/>
+    <mergeCell ref="U6:U11"/>
+    <mergeCell ref="U12:U16"/>
+    <mergeCell ref="P4:P5"/>
+    <mergeCell ref="Q4:Q5"/>
+    <mergeCell ref="R4:R5"/>
+    <mergeCell ref="S4:S5"/>
+    <mergeCell ref="U4:U5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3497,41 +3497,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="74"/>
-      <c r="B1" s="74"/>
-      <c r="C1" s="74"/>
-      <c r="D1" s="74"/>
-      <c r="E1" s="74"/>
-      <c r="F1" s="74"/>
-      <c r="G1" s="74"/>
-      <c r="H1" s="74"/>
-      <c r="I1" s="74"/>
-      <c r="J1" s="74"/>
-      <c r="K1" s="74"/>
-      <c r="L1" s="74"/>
-      <c r="M1" s="74"/>
-      <c r="N1" s="74"/>
-      <c r="O1" s="74"/>
-      <c r="P1" s="74"/>
-      <c r="Q1" s="74"/>
-      <c r="R1" s="74"/>
-      <c r="S1" s="74"/>
-      <c r="T1" s="74"/>
-      <c r="U1" s="74"/>
-      <c r="V1" s="74"/>
+      <c r="A1" s="82"/>
+      <c r="B1" s="82"/>
+      <c r="C1" s="82"/>
+      <c r="D1" s="82"/>
+      <c r="E1" s="82"/>
+      <c r="F1" s="82"/>
+      <c r="G1" s="82"/>
+      <c r="H1" s="82"/>
+      <c r="I1" s="82"/>
+      <c r="J1" s="82"/>
+      <c r="K1" s="82"/>
+      <c r="L1" s="82"/>
+      <c r="M1" s="82"/>
+      <c r="N1" s="82"/>
+      <c r="O1" s="82"/>
+      <c r="P1" s="82"/>
+      <c r="Q1" s="82"/>
+      <c r="R1" s="82"/>
+      <c r="S1" s="82"/>
+      <c r="T1" s="82"/>
+      <c r="U1" s="82"/>
+      <c r="V1" s="82"/>
       <c r="W1" s="44"/>
     </row>
     <row r="2" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="75" t="s">
+      <c r="A2" s="83" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="76"/>
-      <c r="C2" s="76"/>
-      <c r="D2" s="76"/>
-      <c r="E2" s="77" t="s">
+      <c r="B2" s="84"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="85" t="s">
         <v>63</v>
       </c>
-      <c r="F2" s="77"/>
+      <c r="F2" s="85"/>
       <c r="G2" s="4"/>
       <c r="H2" s="20"/>
       <c r="I2" s="48"/>
@@ -3576,58 +3576,58 @@
       <c r="W3" s="26"/>
     </row>
     <row r="4" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="78" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="73" t="s">
+      <c r="A4" s="86" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="81" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="73"/>
-      <c r="D4" s="73"/>
-      <c r="E4" s="73"/>
-      <c r="F4" s="73"/>
-      <c r="G4" s="73"/>
-      <c r="H4" s="73"/>
-      <c r="I4" s="73"/>
-      <c r="J4" s="73" t="s">
+      <c r="C4" s="81"/>
+      <c r="D4" s="81"/>
+      <c r="E4" s="81"/>
+      <c r="F4" s="81"/>
+      <c r="G4" s="81"/>
+      <c r="H4" s="81"/>
+      <c r="I4" s="81"/>
+      <c r="J4" s="81" t="s">
         <v>6</v>
       </c>
-      <c r="K4" s="73" t="s">
+      <c r="K4" s="81" t="s">
         <v>11</v>
       </c>
-      <c r="L4" s="73"/>
-      <c r="M4" s="79" t="s">
+      <c r="L4" s="81"/>
+      <c r="M4" s="78" t="s">
         <v>42</v>
       </c>
-      <c r="N4" s="79" t="s">
+      <c r="N4" s="78" t="s">
         <v>10</v>
       </c>
-      <c r="O4" s="79" t="s">
+      <c r="O4" s="78" t="s">
         <v>7</v>
       </c>
-      <c r="P4" s="84" t="s">
+      <c r="P4" s="76" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="79" t="s">
+      <c r="Q4" s="78" t="s">
         <v>39</v>
       </c>
-      <c r="R4" s="79" t="s">
+      <c r="R4" s="78" t="s">
         <v>53</v>
       </c>
-      <c r="S4" s="86" t="s">
+      <c r="S4" s="80" t="s">
         <v>54</v>
       </c>
       <c r="T4" s="26"/>
-      <c r="U4" s="73" t="s">
+      <c r="U4" s="81" t="s">
         <v>39</v>
       </c>
-      <c r="V4" s="73" t="s">
+      <c r="V4" s="81" t="s">
         <v>53</v>
       </c>
       <c r="W4" s="45"/>
     </row>
     <row r="5" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="78"/>
+      <c r="A5" s="86"/>
       <c r="B5" s="69" t="s">
         <v>1</v>
       </c>
@@ -3652,23 +3652,23 @@
       <c r="I5" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="73"/>
+      <c r="J5" s="81"/>
       <c r="K5" s="69" t="s">
         <v>12</v>
       </c>
       <c r="L5" s="69" t="s">
         <v>13</v>
       </c>
-      <c r="M5" s="80"/>
-      <c r="N5" s="80"/>
-      <c r="O5" s="80"/>
-      <c r="P5" s="85"/>
-      <c r="Q5" s="80"/>
-      <c r="R5" s="80"/>
-      <c r="S5" s="86"/>
+      <c r="M5" s="79"/>
+      <c r="N5" s="79"/>
+      <c r="O5" s="79"/>
+      <c r="P5" s="77"/>
+      <c r="Q5" s="79"/>
+      <c r="R5" s="79"/>
+      <c r="S5" s="80"/>
       <c r="T5" s="26"/>
-      <c r="U5" s="73"/>
-      <c r="V5" s="73"/>
+      <c r="U5" s="81"/>
+      <c r="V5" s="81"/>
       <c r="W5" s="45"/>
     </row>
     <row r="6" spans="1:23" s="11" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -3722,7 +3722,7 @@
       </c>
       <c r="S6" s="67"/>
       <c r="T6" s="68"/>
-      <c r="U6" s="81" t="s">
+      <c r="U6" s="73" t="s">
         <v>18</v>
       </c>
       <c r="V6" s="3" t="s">
@@ -3779,7 +3779,7 @@
       </c>
       <c r="S7" s="67"/>
       <c r="T7" s="68"/>
-      <c r="U7" s="82"/>
+      <c r="U7" s="74"/>
       <c r="V7" s="3" t="s">
         <v>35</v>
       </c>
@@ -3834,7 +3834,7 @@
       </c>
       <c r="S8" s="67"/>
       <c r="T8" s="68"/>
-      <c r="U8" s="82"/>
+      <c r="U8" s="74"/>
       <c r="V8" s="3" t="s">
         <v>21</v>
       </c>
@@ -3889,7 +3889,7 @@
       </c>
       <c r="S9" s="67"/>
       <c r="T9" s="68"/>
-      <c r="U9" s="82"/>
+      <c r="U9" s="74"/>
       <c r="V9" s="3" t="s">
         <v>51</v>
       </c>
@@ -3944,7 +3944,7 @@
       </c>
       <c r="S10" s="67"/>
       <c r="T10" s="68"/>
-      <c r="U10" s="82"/>
+      <c r="U10" s="74"/>
       <c r="V10" s="3" t="s">
         <v>31</v>
       </c>
@@ -4001,7 +4001,7 @@
       </c>
       <c r="S11" s="67"/>
       <c r="T11" s="68"/>
-      <c r="U11" s="82"/>
+      <c r="U11" s="74"/>
       <c r="V11" s="3" t="s">
         <v>30</v>
       </c>
@@ -4056,7 +4056,7 @@
       </c>
       <c r="S12" s="67"/>
       <c r="T12" s="68"/>
-      <c r="U12" s="81" t="s">
+      <c r="U12" s="73" t="s">
         <v>19</v>
       </c>
       <c r="V12" s="3" t="s">
@@ -4087,7 +4087,7 @@
       <c r="R13" s="62"/>
       <c r="S13" s="67"/>
       <c r="T13" s="68"/>
-      <c r="U13" s="82"/>
+      <c r="U13" s="74"/>
       <c r="V13" s="3" t="s">
         <v>37</v>
       </c>
@@ -4116,7 +4116,7 @@
       <c r="R14" s="62"/>
       <c r="S14" s="67"/>
       <c r="T14" s="68"/>
-      <c r="U14" s="82"/>
+      <c r="U14" s="74"/>
       <c r="V14" s="3" t="s">
         <v>36</v>
       </c>
@@ -4145,7 +4145,7 @@
       <c r="R15" s="62"/>
       <c r="S15" s="67"/>
       <c r="T15" s="13"/>
-      <c r="U15" s="82"/>
+      <c r="U15" s="74"/>
       <c r="V15" s="3" t="s">
         <v>24</v>
       </c>
@@ -4174,7 +4174,7 @@
       <c r="R16" s="62"/>
       <c r="S16" s="67"/>
       <c r="T16" s="13"/>
-      <c r="U16" s="83"/>
+      <c r="U16" s="75"/>
       <c r="V16" s="3" t="s">
         <v>25</v>
       </c>
@@ -5891,6 +5891,13 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="U6:U11"/>
+    <mergeCell ref="U12:U16"/>
+    <mergeCell ref="P4:P5"/>
+    <mergeCell ref="Q4:Q5"/>
+    <mergeCell ref="R4:R5"/>
+    <mergeCell ref="S4:S5"/>
+    <mergeCell ref="U4:U5"/>
     <mergeCell ref="V4:V5"/>
     <mergeCell ref="A1:V1"/>
     <mergeCell ref="A2:D2"/>
@@ -5902,13 +5909,6 @@
     <mergeCell ref="M4:M5"/>
     <mergeCell ref="N4:N5"/>
     <mergeCell ref="O4:O5"/>
-    <mergeCell ref="U6:U11"/>
-    <mergeCell ref="U12:U16"/>
-    <mergeCell ref="P4:P5"/>
-    <mergeCell ref="Q4:Q5"/>
-    <mergeCell ref="R4:R5"/>
-    <mergeCell ref="S4:S5"/>
-    <mergeCell ref="U4:U5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5952,41 +5952,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="74"/>
-      <c r="B1" s="74"/>
-      <c r="C1" s="74"/>
-      <c r="D1" s="74"/>
-      <c r="E1" s="74"/>
-      <c r="F1" s="74"/>
-      <c r="G1" s="74"/>
-      <c r="H1" s="74"/>
-      <c r="I1" s="74"/>
-      <c r="J1" s="74"/>
-      <c r="K1" s="74"/>
-      <c r="L1" s="74"/>
-      <c r="M1" s="74"/>
-      <c r="N1" s="74"/>
-      <c r="O1" s="74"/>
-      <c r="P1" s="74"/>
-      <c r="Q1" s="74"/>
-      <c r="R1" s="74"/>
-      <c r="S1" s="74"/>
-      <c r="T1" s="74"/>
-      <c r="U1" s="74"/>
-      <c r="V1" s="74"/>
+      <c r="A1" s="82"/>
+      <c r="B1" s="82"/>
+      <c r="C1" s="82"/>
+      <c r="D1" s="82"/>
+      <c r="E1" s="82"/>
+      <c r="F1" s="82"/>
+      <c r="G1" s="82"/>
+      <c r="H1" s="82"/>
+      <c r="I1" s="82"/>
+      <c r="J1" s="82"/>
+      <c r="K1" s="82"/>
+      <c r="L1" s="82"/>
+      <c r="M1" s="82"/>
+      <c r="N1" s="82"/>
+      <c r="O1" s="82"/>
+      <c r="P1" s="82"/>
+      <c r="Q1" s="82"/>
+      <c r="R1" s="82"/>
+      <c r="S1" s="82"/>
+      <c r="T1" s="82"/>
+      <c r="U1" s="82"/>
+      <c r="V1" s="82"/>
       <c r="W1" s="44"/>
     </row>
     <row r="2" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="75" t="s">
+      <c r="A2" s="83" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="76"/>
-      <c r="C2" s="76"/>
-      <c r="D2" s="76"/>
-      <c r="E2" s="77" t="s">
+      <c r="B2" s="84"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="85" t="s">
         <v>63</v>
       </c>
-      <c r="F2" s="77"/>
+      <c r="F2" s="85"/>
       <c r="G2" s="4"/>
       <c r="H2" s="20"/>
       <c r="I2" s="48"/>
@@ -6031,58 +6031,58 @@
       <c r="W3" s="26"/>
     </row>
     <row r="4" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="78" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="73" t="s">
+      <c r="A4" s="86" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="81" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="73"/>
-      <c r="D4" s="73"/>
-      <c r="E4" s="73"/>
-      <c r="F4" s="73"/>
-      <c r="G4" s="73"/>
-      <c r="H4" s="73"/>
-      <c r="I4" s="73"/>
-      <c r="J4" s="73" t="s">
+      <c r="C4" s="81"/>
+      <c r="D4" s="81"/>
+      <c r="E4" s="81"/>
+      <c r="F4" s="81"/>
+      <c r="G4" s="81"/>
+      <c r="H4" s="81"/>
+      <c r="I4" s="81"/>
+      <c r="J4" s="81" t="s">
         <v>6</v>
       </c>
-      <c r="K4" s="73" t="s">
+      <c r="K4" s="81" t="s">
         <v>11</v>
       </c>
-      <c r="L4" s="73"/>
-      <c r="M4" s="79" t="s">
+      <c r="L4" s="81"/>
+      <c r="M4" s="78" t="s">
         <v>42</v>
       </c>
-      <c r="N4" s="79" t="s">
+      <c r="N4" s="78" t="s">
         <v>10</v>
       </c>
-      <c r="O4" s="79" t="s">
+      <c r="O4" s="78" t="s">
         <v>7</v>
       </c>
-      <c r="P4" s="84" t="s">
+      <c r="P4" s="76" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="79" t="s">
+      <c r="Q4" s="78" t="s">
         <v>39</v>
       </c>
-      <c r="R4" s="79" t="s">
+      <c r="R4" s="78" t="s">
         <v>53</v>
       </c>
-      <c r="S4" s="86" t="s">
+      <c r="S4" s="80" t="s">
         <v>54</v>
       </c>
       <c r="T4" s="26"/>
-      <c r="U4" s="73" t="s">
+      <c r="U4" s="81" t="s">
         <v>39</v>
       </c>
-      <c r="V4" s="73" t="s">
+      <c r="V4" s="81" t="s">
         <v>53</v>
       </c>
       <c r="W4" s="45"/>
     </row>
     <row r="5" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="78"/>
+      <c r="A5" s="86"/>
       <c r="B5" s="56" t="s">
         <v>1</v>
       </c>
@@ -6107,23 +6107,23 @@
       <c r="I5" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="73"/>
+      <c r="J5" s="81"/>
       <c r="K5" s="56" t="s">
         <v>12</v>
       </c>
       <c r="L5" s="56" t="s">
         <v>13</v>
       </c>
-      <c r="M5" s="80"/>
-      <c r="N5" s="80"/>
-      <c r="O5" s="80"/>
-      <c r="P5" s="85"/>
-      <c r="Q5" s="80"/>
-      <c r="R5" s="80"/>
-      <c r="S5" s="86"/>
+      <c r="M5" s="79"/>
+      <c r="N5" s="79"/>
+      <c r="O5" s="79"/>
+      <c r="P5" s="77"/>
+      <c r="Q5" s="79"/>
+      <c r="R5" s="79"/>
+      <c r="S5" s="80"/>
       <c r="T5" s="26"/>
-      <c r="U5" s="73"/>
-      <c r="V5" s="73"/>
+      <c r="U5" s="81"/>
+      <c r="V5" s="81"/>
       <c r="W5" s="45"/>
     </row>
     <row r="6" spans="1:23" s="11" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -6171,7 +6171,7 @@
       </c>
       <c r="S6" s="67"/>
       <c r="T6" s="55"/>
-      <c r="U6" s="81" t="s">
+      <c r="U6" s="73" t="s">
         <v>18</v>
       </c>
       <c r="V6" s="3" t="s">
@@ -6202,7 +6202,7 @@
       <c r="R7" s="62"/>
       <c r="S7" s="67"/>
       <c r="T7" s="55"/>
-      <c r="U7" s="82"/>
+      <c r="U7" s="74"/>
       <c r="V7" s="3" t="s">
         <v>35</v>
       </c>
@@ -6231,7 +6231,7 @@
       <c r="R8" s="62"/>
       <c r="S8" s="67"/>
       <c r="T8" s="55"/>
-      <c r="U8" s="82"/>
+      <c r="U8" s="74"/>
       <c r="V8" s="3" t="s">
         <v>21</v>
       </c>
@@ -6260,7 +6260,7 @@
       <c r="R9" s="62"/>
       <c r="S9" s="67"/>
       <c r="T9" s="55"/>
-      <c r="U9" s="82"/>
+      <c r="U9" s="74"/>
       <c r="V9" s="3" t="s">
         <v>51</v>
       </c>
@@ -6289,7 +6289,7 @@
       <c r="R10" s="62"/>
       <c r="S10" s="67"/>
       <c r="T10" s="55"/>
-      <c r="U10" s="82"/>
+      <c r="U10" s="74"/>
       <c r="V10" s="3" t="s">
         <v>31</v>
       </c>
@@ -6318,7 +6318,7 @@
       <c r="R11" s="62"/>
       <c r="S11" s="67"/>
       <c r="T11" s="55"/>
-      <c r="U11" s="82"/>
+      <c r="U11" s="74"/>
       <c r="V11" s="3" t="s">
         <v>30</v>
       </c>
@@ -6347,7 +6347,7 @@
       <c r="R12" s="62"/>
       <c r="S12" s="67"/>
       <c r="T12" s="55"/>
-      <c r="U12" s="81" t="s">
+      <c r="U12" s="73" t="s">
         <v>19</v>
       </c>
       <c r="V12" s="3" t="s">
@@ -6378,7 +6378,7 @@
       <c r="R13" s="62"/>
       <c r="S13" s="67"/>
       <c r="T13" s="55"/>
-      <c r="U13" s="82"/>
+      <c r="U13" s="74"/>
       <c r="V13" s="3" t="s">
         <v>37</v>
       </c>
@@ -6407,7 +6407,7 @@
       <c r="R14" s="62"/>
       <c r="S14" s="67"/>
       <c r="T14" s="55"/>
-      <c r="U14" s="82"/>
+      <c r="U14" s="74"/>
       <c r="V14" s="3" t="s">
         <v>36</v>
       </c>
@@ -6436,7 +6436,7 @@
       <c r="R15" s="62"/>
       <c r="S15" s="67"/>
       <c r="T15" s="13"/>
-      <c r="U15" s="82"/>
+      <c r="U15" s="74"/>
       <c r="V15" s="3" t="s">
         <v>24</v>
       </c>
@@ -6465,7 +6465,7 @@
       <c r="R16" s="62"/>
       <c r="S16" s="67"/>
       <c r="T16" s="13"/>
-      <c r="U16" s="83"/>
+      <c r="U16" s="75"/>
       <c r="V16" s="3" t="s">
         <v>25</v>
       </c>
@@ -8182,13 +8182,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="U6:U11"/>
-    <mergeCell ref="U12:U16"/>
-    <mergeCell ref="P4:P5"/>
-    <mergeCell ref="Q4:Q5"/>
-    <mergeCell ref="R4:R5"/>
-    <mergeCell ref="S4:S5"/>
-    <mergeCell ref="U4:U5"/>
     <mergeCell ref="V4:V5"/>
     <mergeCell ref="A1:V1"/>
     <mergeCell ref="A2:D2"/>
@@ -8200,6 +8193,13 @@
     <mergeCell ref="M4:M5"/>
     <mergeCell ref="N4:N5"/>
     <mergeCell ref="O4:O5"/>
+    <mergeCell ref="U6:U11"/>
+    <mergeCell ref="U12:U16"/>
+    <mergeCell ref="P4:P5"/>
+    <mergeCell ref="Q4:Q5"/>
+    <mergeCell ref="R4:R5"/>
+    <mergeCell ref="S4:S5"/>
+    <mergeCell ref="U4:U5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -8243,41 +8243,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="74"/>
-      <c r="B1" s="74"/>
-      <c r="C1" s="74"/>
-      <c r="D1" s="74"/>
-      <c r="E1" s="74"/>
-      <c r="F1" s="74"/>
-      <c r="G1" s="74"/>
-      <c r="H1" s="74"/>
-      <c r="I1" s="74"/>
-      <c r="J1" s="74"/>
-      <c r="K1" s="74"/>
-      <c r="L1" s="74"/>
-      <c r="M1" s="74"/>
-      <c r="N1" s="74"/>
-      <c r="O1" s="74"/>
-      <c r="P1" s="74"/>
-      <c r="Q1" s="74"/>
-      <c r="R1" s="74"/>
-      <c r="S1" s="74"/>
-      <c r="T1" s="74"/>
-      <c r="U1" s="74"/>
-      <c r="V1" s="74"/>
+      <c r="A1" s="82"/>
+      <c r="B1" s="82"/>
+      <c r="C1" s="82"/>
+      <c r="D1" s="82"/>
+      <c r="E1" s="82"/>
+      <c r="F1" s="82"/>
+      <c r="G1" s="82"/>
+      <c r="H1" s="82"/>
+      <c r="I1" s="82"/>
+      <c r="J1" s="82"/>
+      <c r="K1" s="82"/>
+      <c r="L1" s="82"/>
+      <c r="M1" s="82"/>
+      <c r="N1" s="82"/>
+      <c r="O1" s="82"/>
+      <c r="P1" s="82"/>
+      <c r="Q1" s="82"/>
+      <c r="R1" s="82"/>
+      <c r="S1" s="82"/>
+      <c r="T1" s="82"/>
+      <c r="U1" s="82"/>
+      <c r="V1" s="82"/>
       <c r="W1" s="44"/>
     </row>
     <row r="2" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="75" t="s">
+      <c r="A2" s="83" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="76"/>
-      <c r="C2" s="76"/>
-      <c r="D2" s="76"/>
-      <c r="E2" s="77" t="s">
+      <c r="B2" s="84"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="85" t="s">
         <v>63</v>
       </c>
-      <c r="F2" s="77"/>
+      <c r="F2" s="85"/>
       <c r="G2" s="4"/>
       <c r="H2" s="20"/>
       <c r="I2" s="48"/>
@@ -8322,58 +8322,58 @@
       <c r="W3" s="26"/>
     </row>
     <row r="4" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="78" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="73" t="s">
+      <c r="A4" s="86" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="81" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="73"/>
-      <c r="D4" s="73"/>
-      <c r="E4" s="73"/>
-      <c r="F4" s="73"/>
-      <c r="G4" s="73"/>
-      <c r="H4" s="73"/>
-      <c r="I4" s="73"/>
-      <c r="J4" s="73" t="s">
+      <c r="C4" s="81"/>
+      <c r="D4" s="81"/>
+      <c r="E4" s="81"/>
+      <c r="F4" s="81"/>
+      <c r="G4" s="81"/>
+      <c r="H4" s="81"/>
+      <c r="I4" s="81"/>
+      <c r="J4" s="81" t="s">
         <v>6</v>
       </c>
-      <c r="K4" s="73" t="s">
+      <c r="K4" s="81" t="s">
         <v>11</v>
       </c>
-      <c r="L4" s="73"/>
-      <c r="M4" s="79" t="s">
+      <c r="L4" s="81"/>
+      <c r="M4" s="78" t="s">
         <v>42</v>
       </c>
-      <c r="N4" s="79" t="s">
+      <c r="N4" s="78" t="s">
         <v>10</v>
       </c>
-      <c r="O4" s="79" t="s">
+      <c r="O4" s="78" t="s">
         <v>7</v>
       </c>
-      <c r="P4" s="84" t="s">
+      <c r="P4" s="76" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="79" t="s">
+      <c r="Q4" s="78" t="s">
         <v>39</v>
       </c>
-      <c r="R4" s="79" t="s">
+      <c r="R4" s="78" t="s">
         <v>53</v>
       </c>
-      <c r="S4" s="86" t="s">
+      <c r="S4" s="80" t="s">
         <v>54</v>
       </c>
       <c r="T4" s="26"/>
-      <c r="U4" s="73" t="s">
+      <c r="U4" s="81" t="s">
         <v>39</v>
       </c>
-      <c r="V4" s="73" t="s">
+      <c r="V4" s="81" t="s">
         <v>53</v>
       </c>
       <c r="W4" s="45"/>
     </row>
     <row r="5" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="78"/>
+      <c r="A5" s="86"/>
       <c r="B5" s="63" t="s">
         <v>1</v>
       </c>
@@ -8398,23 +8398,23 @@
       <c r="I5" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="73"/>
+      <c r="J5" s="81"/>
       <c r="K5" s="63" t="s">
         <v>12</v>
       </c>
       <c r="L5" s="63" t="s">
         <v>13</v>
       </c>
-      <c r="M5" s="80"/>
-      <c r="N5" s="80"/>
-      <c r="O5" s="80"/>
-      <c r="P5" s="85"/>
-      <c r="Q5" s="80"/>
-      <c r="R5" s="80"/>
-      <c r="S5" s="86"/>
+      <c r="M5" s="79"/>
+      <c r="N5" s="79"/>
+      <c r="O5" s="79"/>
+      <c r="P5" s="77"/>
+      <c r="Q5" s="79"/>
+      <c r="R5" s="79"/>
+      <c r="S5" s="80"/>
       <c r="T5" s="26"/>
-      <c r="U5" s="73"/>
-      <c r="V5" s="73"/>
+      <c r="U5" s="81"/>
+      <c r="V5" s="81"/>
       <c r="W5" s="45"/>
     </row>
     <row r="6" spans="1:23" s="11" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -8464,7 +8464,7 @@
       </c>
       <c r="S6" s="67"/>
       <c r="T6" s="64"/>
-      <c r="U6" s="81" t="s">
+      <c r="U6" s="73" t="s">
         <v>18</v>
       </c>
       <c r="V6" s="3" t="s">
@@ -8523,7 +8523,7 @@
       </c>
       <c r="S7" s="67"/>
       <c r="T7" s="64"/>
-      <c r="U7" s="82"/>
+      <c r="U7" s="74"/>
       <c r="V7" s="3" t="s">
         <v>35</v>
       </c>
@@ -8580,7 +8580,7 @@
       </c>
       <c r="S8" s="67"/>
       <c r="T8" s="64"/>
-      <c r="U8" s="82"/>
+      <c r="U8" s="74"/>
       <c r="V8" s="3" t="s">
         <v>21</v>
       </c>
@@ -8633,7 +8633,7 @@
       </c>
       <c r="S9" s="67"/>
       <c r="T9" s="64"/>
-      <c r="U9" s="82"/>
+      <c r="U9" s="74"/>
       <c r="V9" s="3" t="s">
         <v>51</v>
       </c>
@@ -8690,7 +8690,7 @@
       </c>
       <c r="S10" s="67"/>
       <c r="T10" s="64"/>
-      <c r="U10" s="82"/>
+      <c r="U10" s="74"/>
       <c r="V10" s="3" t="s">
         <v>31</v>
       </c>
@@ -8719,7 +8719,7 @@
       <c r="R11" s="62"/>
       <c r="S11" s="67"/>
       <c r="T11" s="64"/>
-      <c r="U11" s="82"/>
+      <c r="U11" s="74"/>
       <c r="V11" s="3" t="s">
         <v>30</v>
       </c>
@@ -8748,7 +8748,7 @@
       <c r="R12" s="62"/>
       <c r="S12" s="67"/>
       <c r="T12" s="64"/>
-      <c r="U12" s="81" t="s">
+      <c r="U12" s="73" t="s">
         <v>19</v>
       </c>
       <c r="V12" s="3" t="s">
@@ -8779,7 +8779,7 @@
       <c r="R13" s="62"/>
       <c r="S13" s="67"/>
       <c r="T13" s="64"/>
-      <c r="U13" s="82"/>
+      <c r="U13" s="74"/>
       <c r="V13" s="3" t="s">
         <v>37</v>
       </c>
@@ -8808,7 +8808,7 @@
       <c r="R14" s="62"/>
       <c r="S14" s="67"/>
       <c r="T14" s="64"/>
-      <c r="U14" s="82"/>
+      <c r="U14" s="74"/>
       <c r="V14" s="3" t="s">
         <v>36</v>
       </c>
@@ -8837,7 +8837,7 @@
       <c r="R15" s="62"/>
       <c r="S15" s="67"/>
       <c r="T15" s="13"/>
-      <c r="U15" s="82"/>
+      <c r="U15" s="74"/>
       <c r="V15" s="3" t="s">
         <v>24</v>
       </c>
@@ -8866,7 +8866,7 @@
       <c r="R16" s="62"/>
       <c r="S16" s="67"/>
       <c r="T16" s="13"/>
-      <c r="U16" s="83"/>
+      <c r="U16" s="75"/>
       <c r="V16" s="3" t="s">
         <v>25</v>
       </c>
@@ -10583,13 +10583,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="U6:U11"/>
-    <mergeCell ref="U12:U16"/>
-    <mergeCell ref="P4:P5"/>
-    <mergeCell ref="Q4:Q5"/>
-    <mergeCell ref="R4:R5"/>
-    <mergeCell ref="S4:S5"/>
-    <mergeCell ref="U4:U5"/>
     <mergeCell ref="V4:V5"/>
     <mergeCell ref="A1:V1"/>
     <mergeCell ref="A2:D2"/>
@@ -10601,6 +10594,13 @@
     <mergeCell ref="M4:M5"/>
     <mergeCell ref="N4:N5"/>
     <mergeCell ref="O4:O5"/>
+    <mergeCell ref="U6:U11"/>
+    <mergeCell ref="U12:U16"/>
+    <mergeCell ref="P4:P5"/>
+    <mergeCell ref="Q4:Q5"/>
+    <mergeCell ref="R4:R5"/>
+    <mergeCell ref="S4:S5"/>
+    <mergeCell ref="U4:U5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -10644,41 +10644,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="74"/>
-      <c r="B1" s="74"/>
-      <c r="C1" s="74"/>
-      <c r="D1" s="74"/>
-      <c r="E1" s="74"/>
-      <c r="F1" s="74"/>
-      <c r="G1" s="74"/>
-      <c r="H1" s="74"/>
-      <c r="I1" s="74"/>
-      <c r="J1" s="74"/>
-      <c r="K1" s="74"/>
-      <c r="L1" s="74"/>
-      <c r="M1" s="74"/>
-      <c r="N1" s="74"/>
-      <c r="O1" s="74"/>
-      <c r="P1" s="74"/>
-      <c r="Q1" s="74"/>
-      <c r="R1" s="74"/>
-      <c r="S1" s="74"/>
-      <c r="T1" s="74"/>
-      <c r="U1" s="74"/>
-      <c r="V1" s="74"/>
+      <c r="A1" s="82"/>
+      <c r="B1" s="82"/>
+      <c r="C1" s="82"/>
+      <c r="D1" s="82"/>
+      <c r="E1" s="82"/>
+      <c r="F1" s="82"/>
+      <c r="G1" s="82"/>
+      <c r="H1" s="82"/>
+      <c r="I1" s="82"/>
+      <c r="J1" s="82"/>
+      <c r="K1" s="82"/>
+      <c r="L1" s="82"/>
+      <c r="M1" s="82"/>
+      <c r="N1" s="82"/>
+      <c r="O1" s="82"/>
+      <c r="P1" s="82"/>
+      <c r="Q1" s="82"/>
+      <c r="R1" s="82"/>
+      <c r="S1" s="82"/>
+      <c r="T1" s="82"/>
+      <c r="U1" s="82"/>
+      <c r="V1" s="82"/>
       <c r="W1" s="44"/>
     </row>
     <row r="2" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="75" t="s">
+      <c r="A2" s="83" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="76"/>
-      <c r="C2" s="76"/>
-      <c r="D2" s="76"/>
-      <c r="E2" s="77" t="s">
+      <c r="B2" s="84"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="85" t="s">
         <v>63</v>
       </c>
-      <c r="F2" s="77"/>
+      <c r="F2" s="85"/>
       <c r="G2" s="4"/>
       <c r="H2" s="20"/>
       <c r="I2" s="48"/>
@@ -10723,58 +10723,58 @@
       <c r="W3" s="26"/>
     </row>
     <row r="4" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="78" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="73" t="s">
+      <c r="A4" s="86" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="81" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="73"/>
-      <c r="D4" s="73"/>
-      <c r="E4" s="73"/>
-      <c r="F4" s="73"/>
-      <c r="G4" s="73"/>
-      <c r="H4" s="73"/>
-      <c r="I4" s="73"/>
-      <c r="J4" s="73" t="s">
+      <c r="C4" s="81"/>
+      <c r="D4" s="81"/>
+      <c r="E4" s="81"/>
+      <c r="F4" s="81"/>
+      <c r="G4" s="81"/>
+      <c r="H4" s="81"/>
+      <c r="I4" s="81"/>
+      <c r="J4" s="81" t="s">
         <v>6</v>
       </c>
-      <c r="K4" s="73" t="s">
+      <c r="K4" s="81" t="s">
         <v>11</v>
       </c>
-      <c r="L4" s="73"/>
-      <c r="M4" s="79" t="s">
+      <c r="L4" s="81"/>
+      <c r="M4" s="78" t="s">
         <v>42</v>
       </c>
-      <c r="N4" s="79" t="s">
+      <c r="N4" s="78" t="s">
         <v>10</v>
       </c>
-      <c r="O4" s="79" t="s">
+      <c r="O4" s="78" t="s">
         <v>7</v>
       </c>
-      <c r="P4" s="84" t="s">
+      <c r="P4" s="76" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="79" t="s">
+      <c r="Q4" s="78" t="s">
         <v>39</v>
       </c>
-      <c r="R4" s="79" t="s">
+      <c r="R4" s="78" t="s">
         <v>53</v>
       </c>
-      <c r="S4" s="86" t="s">
+      <c r="S4" s="80" t="s">
         <v>54</v>
       </c>
       <c r="T4" s="26"/>
-      <c r="U4" s="73" t="s">
+      <c r="U4" s="81" t="s">
         <v>39</v>
       </c>
-      <c r="V4" s="73" t="s">
+      <c r="V4" s="81" t="s">
         <v>53</v>
       </c>
       <c r="W4" s="45"/>
     </row>
     <row r="5" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="78"/>
+      <c r="A5" s="86"/>
       <c r="B5" s="63" t="s">
         <v>1</v>
       </c>
@@ -10799,23 +10799,23 @@
       <c r="I5" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="73"/>
+      <c r="J5" s="81"/>
       <c r="K5" s="63" t="s">
         <v>12</v>
       </c>
       <c r="L5" s="63" t="s">
         <v>13</v>
       </c>
-      <c r="M5" s="80"/>
-      <c r="N5" s="80"/>
-      <c r="O5" s="80"/>
-      <c r="P5" s="85"/>
-      <c r="Q5" s="80"/>
-      <c r="R5" s="80"/>
-      <c r="S5" s="86"/>
+      <c r="M5" s="79"/>
+      <c r="N5" s="79"/>
+      <c r="O5" s="79"/>
+      <c r="P5" s="77"/>
+      <c r="Q5" s="79"/>
+      <c r="R5" s="79"/>
+      <c r="S5" s="80"/>
       <c r="T5" s="26"/>
-      <c r="U5" s="73"/>
-      <c r="V5" s="73"/>
+      <c r="U5" s="81"/>
+      <c r="V5" s="81"/>
       <c r="W5" s="45"/>
     </row>
     <row r="6" spans="1:23" s="11" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -10863,7 +10863,7 @@
       </c>
       <c r="S6" s="67"/>
       <c r="T6" s="64"/>
-      <c r="U6" s="81" t="s">
+      <c r="U6" s="73" t="s">
         <v>18</v>
       </c>
       <c r="V6" s="3" t="s">
@@ -10916,7 +10916,7 @@
       </c>
       <c r="S7" s="67"/>
       <c r="T7" s="64"/>
-      <c r="U7" s="82"/>
+      <c r="U7" s="74"/>
       <c r="V7" s="3" t="s">
         <v>35</v>
       </c>
@@ -10945,7 +10945,7 @@
       <c r="R8" s="62"/>
       <c r="S8" s="67"/>
       <c r="T8" s="64"/>
-      <c r="U8" s="82"/>
+      <c r="U8" s="74"/>
       <c r="V8" s="3" t="s">
         <v>21</v>
       </c>
@@ -10974,7 +10974,7 @@
       <c r="R9" s="62"/>
       <c r="S9" s="67"/>
       <c r="T9" s="64"/>
-      <c r="U9" s="82"/>
+      <c r="U9" s="74"/>
       <c r="V9" s="3" t="s">
         <v>51</v>
       </c>
@@ -11003,7 +11003,7 @@
       <c r="R10" s="62"/>
       <c r="S10" s="67"/>
       <c r="T10" s="64"/>
-      <c r="U10" s="82"/>
+      <c r="U10" s="74"/>
       <c r="V10" s="3" t="s">
         <v>31</v>
       </c>
@@ -11032,7 +11032,7 @@
       <c r="R11" s="62"/>
       <c r="S11" s="67"/>
       <c r="T11" s="64"/>
-      <c r="U11" s="82"/>
+      <c r="U11" s="74"/>
       <c r="V11" s="3" t="s">
         <v>30</v>
       </c>
@@ -11061,7 +11061,7 @@
       <c r="R12" s="62"/>
       <c r="S12" s="67"/>
       <c r="T12" s="64"/>
-      <c r="U12" s="81" t="s">
+      <c r="U12" s="73" t="s">
         <v>19</v>
       </c>
       <c r="V12" s="3" t="s">
@@ -11092,7 +11092,7 @@
       <c r="R13" s="62"/>
       <c r="S13" s="67"/>
       <c r="T13" s="64"/>
-      <c r="U13" s="82"/>
+      <c r="U13" s="74"/>
       <c r="V13" s="3" t="s">
         <v>37</v>
       </c>
@@ -11121,7 +11121,7 @@
       <c r="R14" s="62"/>
       <c r="S14" s="67"/>
       <c r="T14" s="64"/>
-      <c r="U14" s="82"/>
+      <c r="U14" s="74"/>
       <c r="V14" s="3" t="s">
         <v>36</v>
       </c>
@@ -11150,7 +11150,7 @@
       <c r="R15" s="62"/>
       <c r="S15" s="67"/>
       <c r="T15" s="13"/>
-      <c r="U15" s="82"/>
+      <c r="U15" s="74"/>
       <c r="V15" s="3" t="s">
         <v>24</v>
       </c>
@@ -11179,7 +11179,7 @@
       <c r="R16" s="62"/>
       <c r="S16" s="67"/>
       <c r="T16" s="13"/>
-      <c r="U16" s="83"/>
+      <c r="U16" s="75"/>
       <c r="V16" s="3" t="s">
         <v>25</v>
       </c>
@@ -12896,13 +12896,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="U6:U11"/>
-    <mergeCell ref="U12:U16"/>
-    <mergeCell ref="P4:P5"/>
-    <mergeCell ref="Q4:Q5"/>
-    <mergeCell ref="R4:R5"/>
-    <mergeCell ref="S4:S5"/>
-    <mergeCell ref="U4:U5"/>
     <mergeCell ref="V4:V5"/>
     <mergeCell ref="A1:V1"/>
     <mergeCell ref="A2:D2"/>
@@ -12914,6 +12907,13 @@
     <mergeCell ref="M4:M5"/>
     <mergeCell ref="N4:N5"/>
     <mergeCell ref="O4:O5"/>
+    <mergeCell ref="U6:U11"/>
+    <mergeCell ref="U12:U16"/>
+    <mergeCell ref="P4:P5"/>
+    <mergeCell ref="Q4:Q5"/>
+    <mergeCell ref="R4:R5"/>
+    <mergeCell ref="S4:S5"/>
+    <mergeCell ref="U4:U5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -12957,41 +12957,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="74"/>
-      <c r="B1" s="74"/>
-      <c r="C1" s="74"/>
-      <c r="D1" s="74"/>
-      <c r="E1" s="74"/>
-      <c r="F1" s="74"/>
-      <c r="G1" s="74"/>
-      <c r="H1" s="74"/>
-      <c r="I1" s="74"/>
-      <c r="J1" s="74"/>
-      <c r="K1" s="74"/>
-      <c r="L1" s="74"/>
-      <c r="M1" s="74"/>
-      <c r="N1" s="74"/>
-      <c r="O1" s="74"/>
-      <c r="P1" s="74"/>
-      <c r="Q1" s="74"/>
-      <c r="R1" s="74"/>
-      <c r="S1" s="74"/>
-      <c r="T1" s="74"/>
-      <c r="U1" s="74"/>
-      <c r="V1" s="74"/>
+      <c r="A1" s="82"/>
+      <c r="B1" s="82"/>
+      <c r="C1" s="82"/>
+      <c r="D1" s="82"/>
+      <c r="E1" s="82"/>
+      <c r="F1" s="82"/>
+      <c r="G1" s="82"/>
+      <c r="H1" s="82"/>
+      <c r="I1" s="82"/>
+      <c r="J1" s="82"/>
+      <c r="K1" s="82"/>
+      <c r="L1" s="82"/>
+      <c r="M1" s="82"/>
+      <c r="N1" s="82"/>
+      <c r="O1" s="82"/>
+      <c r="P1" s="82"/>
+      <c r="Q1" s="82"/>
+      <c r="R1" s="82"/>
+      <c r="S1" s="82"/>
+      <c r="T1" s="82"/>
+      <c r="U1" s="82"/>
+      <c r="V1" s="82"/>
       <c r="W1" s="44"/>
     </row>
     <row r="2" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="75" t="s">
+      <c r="A2" s="83" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="76"/>
-      <c r="C2" s="76"/>
-      <c r="D2" s="76"/>
-      <c r="E2" s="77" t="s">
+      <c r="B2" s="84"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="85" t="s">
         <v>63</v>
       </c>
-      <c r="F2" s="77"/>
+      <c r="F2" s="85"/>
       <c r="G2" s="4"/>
       <c r="H2" s="20"/>
       <c r="I2" s="20"/>
@@ -13036,58 +13036,58 @@
       <c r="W3" s="26"/>
     </row>
     <row r="4" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="78" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="73" t="s">
+      <c r="A4" s="86" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="81" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="73"/>
-      <c r="D4" s="73"/>
-      <c r="E4" s="73"/>
-      <c r="F4" s="73"/>
-      <c r="G4" s="73"/>
-      <c r="H4" s="73"/>
-      <c r="I4" s="73"/>
-      <c r="J4" s="73" t="s">
+      <c r="C4" s="81"/>
+      <c r="D4" s="81"/>
+      <c r="E4" s="81"/>
+      <c r="F4" s="81"/>
+      <c r="G4" s="81"/>
+      <c r="H4" s="81"/>
+      <c r="I4" s="81"/>
+      <c r="J4" s="81" t="s">
         <v>6</v>
       </c>
-      <c r="K4" s="73" t="s">
+      <c r="K4" s="81" t="s">
         <v>11</v>
       </c>
-      <c r="L4" s="73"/>
-      <c r="M4" s="79" t="s">
+      <c r="L4" s="81"/>
+      <c r="M4" s="78" t="s">
         <v>42</v>
       </c>
-      <c r="N4" s="79" t="s">
+      <c r="N4" s="78" t="s">
         <v>10</v>
       </c>
-      <c r="O4" s="73" t="s">
+      <c r="O4" s="81" t="s">
         <v>7</v>
       </c>
       <c r="P4" s="87" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="73" t="s">
+      <c r="Q4" s="81" t="s">
         <v>39</v>
       </c>
-      <c r="R4" s="73" t="s">
+      <c r="R4" s="81" t="s">
         <v>53</v>
       </c>
-      <c r="S4" s="86" t="s">
+      <c r="S4" s="80" t="s">
         <v>54</v>
       </c>
       <c r="T4" s="26"/>
-      <c r="U4" s="73" t="s">
+      <c r="U4" s="81" t="s">
         <v>39</v>
       </c>
-      <c r="V4" s="73" t="s">
+      <c r="V4" s="81" t="s">
         <v>53</v>
       </c>
       <c r="W4" s="45"/>
     </row>
     <row r="5" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="78"/>
+      <c r="A5" s="86"/>
       <c r="B5" s="41" t="s">
         <v>1</v>
       </c>
@@ -13112,23 +13112,23 @@
       <c r="I5" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="73"/>
+      <c r="J5" s="81"/>
       <c r="K5" s="41" t="s">
         <v>12</v>
       </c>
       <c r="L5" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="M5" s="80"/>
-      <c r="N5" s="80"/>
-      <c r="O5" s="73"/>
+      <c r="M5" s="79"/>
+      <c r="N5" s="79"/>
+      <c r="O5" s="81"/>
       <c r="P5" s="87"/>
-      <c r="Q5" s="73"/>
-      <c r="R5" s="73"/>
-      <c r="S5" s="86"/>
+      <c r="Q5" s="81"/>
+      <c r="R5" s="81"/>
+      <c r="S5" s="80"/>
       <c r="T5" s="26"/>
-      <c r="U5" s="73"/>
-      <c r="V5" s="73"/>
+      <c r="U5" s="81"/>
+      <c r="V5" s="81"/>
       <c r="W5" s="45"/>
     </row>
     <row r="6" spans="1:23" s="11" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -13154,7 +13154,7 @@
       <c r="R6" s="37"/>
       <c r="S6" s="3"/>
       <c r="T6" s="40"/>
-      <c r="U6" s="81" t="s">
+      <c r="U6" s="73" t="s">
         <v>18</v>
       </c>
       <c r="V6" s="3" t="s">
@@ -13185,7 +13185,7 @@
       <c r="R7" s="37"/>
       <c r="S7" s="3"/>
       <c r="T7" s="40"/>
-      <c r="U7" s="82"/>
+      <c r="U7" s="74"/>
       <c r="V7" s="3" t="s">
         <v>35</v>
       </c>
@@ -13214,7 +13214,7 @@
       <c r="R8" s="37"/>
       <c r="S8" s="3"/>
       <c r="T8" s="40"/>
-      <c r="U8" s="82"/>
+      <c r="U8" s="74"/>
       <c r="V8" s="3" t="s">
         <v>21</v>
       </c>
@@ -13243,7 +13243,7 @@
       <c r="R9" s="37"/>
       <c r="S9" s="3"/>
       <c r="T9" s="40"/>
-      <c r="U9" s="82"/>
+      <c r="U9" s="74"/>
       <c r="V9" s="3" t="s">
         <v>51</v>
       </c>
@@ -13272,7 +13272,7 @@
       <c r="R10" s="37"/>
       <c r="S10" s="3"/>
       <c r="T10" s="40"/>
-      <c r="U10" s="82"/>
+      <c r="U10" s="74"/>
       <c r="V10" s="3" t="s">
         <v>31</v>
       </c>
@@ -13301,7 +13301,7 @@
       <c r="R11" s="37"/>
       <c r="S11" s="3"/>
       <c r="T11" s="40"/>
-      <c r="U11" s="82"/>
+      <c r="U11" s="74"/>
       <c r="V11" s="3" t="s">
         <v>30</v>
       </c>
@@ -13330,7 +13330,7 @@
       <c r="R12" s="37"/>
       <c r="S12" s="3"/>
       <c r="T12" s="40"/>
-      <c r="U12" s="81" t="s">
+      <c r="U12" s="73" t="s">
         <v>19</v>
       </c>
       <c r="V12" s="3" t="s">
@@ -13361,7 +13361,7 @@
       <c r="R13" s="9"/>
       <c r="S13" s="3"/>
       <c r="T13" s="40"/>
-      <c r="U13" s="82"/>
+      <c r="U13" s="74"/>
       <c r="V13" s="3" t="s">
         <v>37</v>
       </c>
@@ -13390,7 +13390,7 @@
       <c r="R14" s="37"/>
       <c r="S14" s="3"/>
       <c r="T14" s="40"/>
-      <c r="U14" s="82"/>
+      <c r="U14" s="74"/>
       <c r="V14" s="3" t="s">
         <v>36</v>
       </c>
@@ -13419,7 +13419,7 @@
       <c r="R15" s="37"/>
       <c r="S15" s="3"/>
       <c r="T15" s="13"/>
-      <c r="U15" s="82"/>
+      <c r="U15" s="74"/>
       <c r="V15" s="3" t="s">
         <v>24</v>
       </c>
@@ -13448,7 +13448,7 @@
       <c r="R16" s="37"/>
       <c r="S16" s="3"/>
       <c r="T16" s="13"/>
-      <c r="U16" s="83"/>
+      <c r="U16" s="75"/>
       <c r="V16" s="3" t="s">
         <v>25</v>
       </c>
@@ -14679,13 +14679,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="U6:U11"/>
-    <mergeCell ref="U12:U16"/>
-    <mergeCell ref="P4:P5"/>
-    <mergeCell ref="Q4:Q5"/>
-    <mergeCell ref="R4:R5"/>
-    <mergeCell ref="S4:S5"/>
-    <mergeCell ref="U4:U5"/>
     <mergeCell ref="V4:V5"/>
     <mergeCell ref="A1:V1"/>
     <mergeCell ref="A2:D2"/>
@@ -14697,6 +14690,13 @@
     <mergeCell ref="M4:M5"/>
     <mergeCell ref="N4:N5"/>
     <mergeCell ref="O4:O5"/>
+    <mergeCell ref="U6:U11"/>
+    <mergeCell ref="U12:U16"/>
+    <mergeCell ref="P4:P5"/>
+    <mergeCell ref="Q4:Q5"/>
+    <mergeCell ref="R4:R5"/>
+    <mergeCell ref="S4:S5"/>
+    <mergeCell ref="U4:U5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>